<commit_message>
email tracking feature added
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="48">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -163,27 +163,6 @@
   </si>
   <si>
     <t>DVl8pCYJ6bUSjWs7</t>
-  </si>
-  <si>
-    <t>Ashlee</t>
-  </si>
-  <si>
-    <t>Cross</t>
-  </si>
-  <si>
-    <t>fasteners360@gmail.com</t>
-  </si>
-  <si>
-    <t>KJoiu(*&amp;%23419$$$IUY</t>
-  </si>
-  <si>
-    <t>81.28.96.172:60742</t>
-  </si>
-  <si>
-    <t>3WGWzEabc7tcRQfZ</t>
-  </si>
-  <si>
-    <t>fwaNRX26D4cb9Uf5</t>
   </si>
 </sst>
 </file>
@@ -990,9 +969,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G11"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1226,29 +1207,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>53</v>
-      </c>
-      <c r="G11" t="s">
-        <v>54</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added failsafe for email body on smtp
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Upwork\2020\gmail_app\gmail_app\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\2020\gmail_app\gmail_app\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -42,202 +42,73 @@
     <t>PROXY_PASS</t>
   </si>
   <si>
-    <t>Elva</t>
-  </si>
-  <si>
-    <t>Lynn</t>
-  </si>
-  <si>
-    <t>Elva.Lynn1987@gmail.com</t>
-  </si>
-  <si>
-    <t>C9nqK4Xz6gbUocjf</t>
-  </si>
-  <si>
-    <t>81.28.96.172:43739</t>
-  </si>
-  <si>
-    <t>a4ZJCKXpyPxqtgAt</t>
-  </si>
-  <si>
-    <t>WZRYymEeVjfQeR6Z</t>
-  </si>
-  <si>
-    <t>Daphne</t>
-  </si>
-  <si>
-    <t>Boone</t>
-  </si>
-  <si>
-    <t>Daphne.Boone2002@gmail.com</t>
-  </si>
-  <si>
-    <t>aPxbySqRts82761Y</t>
-  </si>
-  <si>
-    <t>81.28.96.172:30660</t>
-  </si>
-  <si>
-    <t>Loretta</t>
-  </si>
-  <si>
-    <t>Douglas</t>
-  </si>
-  <si>
-    <t>Loretta.Douglas1999@gmail.com</t>
-  </si>
-  <si>
-    <t>J81VtrwOdF2SGqj6</t>
-  </si>
-  <si>
-    <t>81.28.96.172:41489</t>
-  </si>
-  <si>
-    <t>Rene</t>
-  </si>
-  <si>
-    <t>Huber</t>
-  </si>
-  <si>
-    <t>Rene.Huber1999@gmail.com</t>
-  </si>
-  <si>
-    <t>oL30u8vUSzaRp5kn</t>
-  </si>
-  <si>
-    <t>Paula</t>
-  </si>
-  <si>
-    <t>Robertson</t>
-  </si>
-  <si>
-    <t>Paula.Robertson2000@gmail.com</t>
-  </si>
-  <si>
-    <t>l0wkPivmX2FRsCcW</t>
-  </si>
-  <si>
-    <t>Keri</t>
-  </si>
-  <si>
-    <t>Long</t>
-  </si>
-  <si>
-    <t>Keri.Long1998@gmail.com</t>
-  </si>
-  <si>
-    <t>f0xDq4Xgy3nPoMYc</t>
-  </si>
-  <si>
-    <t>Polly</t>
-  </si>
-  <si>
-    <t>Whitehead</t>
-  </si>
-  <si>
-    <t>Polly.Whitehead1997@gmail.com</t>
-  </si>
-  <si>
-    <t>l8RGLVP17bJ4idAF</t>
-  </si>
-  <si>
-    <t>Anne</t>
-  </si>
-  <si>
-    <t>Carlson</t>
-  </si>
-  <si>
-    <t>Anne.Carlson1999@gmail.com</t>
-  </si>
-  <si>
-    <t>BwOdRHpL503bueZC</t>
-  </si>
-  <si>
-    <t>Aurelia</t>
-  </si>
-  <si>
-    <t>Rodriquez</t>
-  </si>
-  <si>
-    <t>Aurelia.Rodriquez1995@gmail.com</t>
-  </si>
-  <si>
-    <t>DVl8pCYJ6bUSjWs7</t>
-  </si>
-  <si>
-    <t>Courtney</t>
-  </si>
-  <si>
-    <t>Holcomb</t>
-  </si>
-  <si>
-    <t>Courtney.Holcomb.1992@gmail.com</t>
-  </si>
-  <si>
-    <t>J90PAVtH85i1vC2h</t>
-  </si>
-  <si>
-    <t>81.28.96.172:15878</t>
-  </si>
-  <si>
-    <t>Jill</t>
-  </si>
-  <si>
-    <t>Middleton</t>
-  </si>
-  <si>
-    <t>Jill.Middleton.1980@gmail.com</t>
-  </si>
-  <si>
-    <t>QkserjiJNZGdu5WF</t>
-  </si>
-  <si>
-    <t>81.28.96.172:65448</t>
-  </si>
-  <si>
-    <t>Justine</t>
-  </si>
-  <si>
-    <t>Lester</t>
-  </si>
-  <si>
-    <t>Justine.Lester.1981@gmail.com</t>
-  </si>
-  <si>
-    <t>DpzEuqQtJsn0l65F</t>
-  </si>
-  <si>
-    <t>81.28.96.172:5596</t>
-  </si>
-  <si>
-    <t>Ola</t>
-  </si>
-  <si>
-    <t>Hampton</t>
-  </si>
-  <si>
-    <t>Ola.Hampton.1982@gmail.com</t>
-  </si>
-  <si>
-    <t>kgQdKfc8IHlw1CWO</t>
-  </si>
-  <si>
-    <t>81.28.96.172:65014</t>
-  </si>
-  <si>
-    <t>Earlene</t>
-  </si>
-  <si>
-    <t>Simon</t>
-  </si>
-  <si>
-    <t>Earlene.Simon.1983@gmail.com</t>
-  </si>
-  <si>
-    <t>qlrLPymGRdcEZo1h</t>
-  </si>
-  <si>
-    <t>81.28.96.172:3222</t>
+    <t>Franklin</t>
+  </si>
+  <si>
+    <t>Logans</t>
+  </si>
+  <si>
+    <t>frankinsonloslogansi@gmail.com</t>
+  </si>
+  <si>
+    <t>kdejqyra</t>
+  </si>
+  <si>
+    <t>185.24.233.182:4006</t>
+  </si>
+  <si>
+    <t>8GbKtEpRUr29jbg5</t>
+  </si>
+  <si>
+    <t>TMwprA4NyqSKxc6V</t>
+  </si>
+  <si>
+    <t>Frederick</t>
+  </si>
+  <si>
+    <t>Salamon</t>
+  </si>
+  <si>
+    <t>fredericksongatsalamon@gmail.com</t>
+  </si>
+  <si>
+    <t>kyqcxzun</t>
+  </si>
+  <si>
+    <t>185.24.233.182:4007</t>
+  </si>
+  <si>
+    <t>Morrison</t>
+  </si>
+  <si>
+    <t>frankinsonleemorison443@gmail.com</t>
+  </si>
+  <si>
+    <t>qzbsvkrp</t>
+  </si>
+  <si>
+    <t>185.24.233.182:4008</t>
+  </si>
+  <si>
+    <t>Vartinson</t>
+  </si>
+  <si>
+    <t>fredriksonkarlosvartinson@gmail.com</t>
+  </si>
+  <si>
+    <t>enpxdtwh</t>
+  </si>
+  <si>
+    <t>185.24.233.182:4009</t>
+  </si>
+  <si>
+    <t>Johnsson</t>
+  </si>
+  <si>
+    <t>frankinsonleejhonson5@gmail.com</t>
+  </si>
+  <si>
+    <t>vznrcpwb</t>
   </si>
 </sst>
 </file>
@@ -1044,10 +915,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11:XFD11"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1123,19 +994,19 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
         <v>19</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>20</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" t="s">
+      <c r="E4" t="s">
         <v>22</v>
-      </c>
-      <c r="E4" t="s">
-        <v>23</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1146,19 +1017,19 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>14</v>
+      </c>
+      <c r="B5" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="B5" t="s">
+      <c r="D5" t="s">
         <v>25</v>
       </c>
-      <c r="C5" t="s">
+      <c r="E5" t="s">
         <v>26</v>
-      </c>
-      <c r="D5" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -1169,231 +1040,24 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
         <v>28</v>
       </c>
-      <c r="B6" t="s">
+      <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="C6" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" t="s">
-        <v>31</v>
-      </c>
       <c r="E6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>32</v>
-      </c>
-      <c r="B7" t="s">
-        <v>33</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>35</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>37</v>
-      </c>
-      <c r="C8" t="s">
-        <v>38</v>
-      </c>
-      <c r="D8" t="s">
-        <v>39</v>
-      </c>
-      <c r="E8" t="s">
-        <v>18</v>
-      </c>
-      <c r="F8" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>40</v>
-      </c>
-      <c r="B9" t="s">
-        <v>41</v>
-      </c>
-      <c r="C9" t="s">
-        <v>42</v>
-      </c>
-      <c r="D9" t="s">
-        <v>43</v>
-      </c>
-      <c r="E9" t="s">
-        <v>23</v>
-      </c>
-      <c r="F9" t="s">
-        <v>12</v>
-      </c>
-      <c r="G9" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" t="s">
-        <v>45</v>
-      </c>
-      <c r="C10" t="s">
-        <v>46</v>
-      </c>
-      <c r="D10" t="s">
-        <v>47</v>
-      </c>
-      <c r="E10" t="s">
-        <v>11</v>
-      </c>
-      <c r="F10" t="s">
-        <v>12</v>
-      </c>
-      <c r="G10" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>48</v>
-      </c>
-      <c r="B11" t="s">
-        <v>49</v>
-      </c>
-      <c r="C11" t="s">
-        <v>50</v>
-      </c>
-      <c r="D11" t="s">
-        <v>51</v>
-      </c>
-      <c r="E11" t="s">
-        <v>52</v>
-      </c>
-      <c r="F11" t="s">
-        <v>12</v>
-      </c>
-      <c r="G11" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>53</v>
-      </c>
-      <c r="B12" t="s">
-        <v>54</v>
-      </c>
-      <c r="C12" t="s">
-        <v>55</v>
-      </c>
-      <c r="D12" t="s">
-        <v>56</v>
-      </c>
-      <c r="E12" t="s">
-        <v>57</v>
-      </c>
-      <c r="F12" t="s">
-        <v>12</v>
-      </c>
-      <c r="G12" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>58</v>
-      </c>
-      <c r="B13" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" t="s">
-        <v>62</v>
-      </c>
-      <c r="F13" t="s">
-        <v>12</v>
-      </c>
-      <c r="G13" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" t="s">
-        <v>64</v>
-      </c>
-      <c r="C14" t="s">
-        <v>65</v>
-      </c>
-      <c r="D14" t="s">
-        <v>66</v>
-      </c>
-      <c r="E14" t="s">
-        <v>67</v>
-      </c>
-      <c r="F14" t="s">
-        <v>12</v>
-      </c>
-      <c r="G14" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>68</v>
-      </c>
-      <c r="B15" t="s">
-        <v>69</v>
-      </c>
-      <c r="C15" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" t="s">
-        <v>71</v>
-      </c>
-      <c r="E15" t="s">
-        <v>72</v>
-      </c>
-      <c r="F15" t="s">
-        <v>12</v>
-      </c>
-      <c r="G15" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
three retries added on smtp class
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34200" windowHeight="11610"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34200" windowHeight="11616"/>
   </bookViews>
   <sheets>
     <sheet name="group_a" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -109,6 +109,21 @@
   </si>
   <si>
     <t>vznrcpwb</t>
+  </si>
+  <si>
+    <t>mrshahimranshovon@gmail.com</t>
+  </si>
+  <si>
+    <t>twg5ZmvBqsixAfr</t>
+  </si>
+  <si>
+    <t>8GbKtEpRUr29jbg6</t>
+  </si>
+  <si>
+    <t>Shah</t>
+  </si>
+  <si>
+    <t>Imran</t>
   </si>
 </sst>
 </file>
@@ -915,15 +930,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="25" customWidth="1"/>
+    <col min="6" max="6" width="32.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -946,44 +965,44 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>33</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>30</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>31</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="G2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
         <v>12</v>
@@ -992,21 +1011,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="F4" t="s">
         <v>12</v>
@@ -1015,21 +1034,21 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="C5" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="D5" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F5" t="s">
         <v>12</v>
@@ -1038,26 +1057,49 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="E6" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>12</v>
       </c>
       <c r="G6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" t="s">
+        <v>27</v>
+      </c>
+      <c r="C7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" t="s">
+        <v>12</v>
+      </c>
+      <c r="G7" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
inbox webhook one by one
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="260">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -42,95 +42,770 @@
     <t>PROXY_PASS</t>
   </si>
   <si>
-    <t>Franklin</t>
-  </si>
-  <si>
-    <t>Logans</t>
-  </si>
-  <si>
-    <t>frankinsonloslogansi@gmail.com</t>
-  </si>
-  <si>
-    <t>kdejqyra</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4006</t>
-  </si>
-  <si>
-    <t>8GbKtEpRUr29jbg5</t>
-  </si>
-  <si>
-    <t>TMwprA4NyqSKxc6V</t>
-  </si>
-  <si>
-    <t>Frederick</t>
-  </si>
-  <si>
-    <t>Salamon</t>
-  </si>
-  <si>
-    <t>fredericksongatsalamon@gmail.com</t>
-  </si>
-  <si>
-    <t>kyqcxzun</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4007</t>
-  </si>
-  <si>
-    <t>Morrison</t>
-  </si>
-  <si>
-    <t>frankinsonleemorison443@gmail.com</t>
-  </si>
-  <si>
-    <t>qzbsvkrp</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4008</t>
-  </si>
-  <si>
-    <t>Vartinson</t>
-  </si>
-  <si>
-    <t>fredriksonkarlosvartinson@gmail.com</t>
-  </si>
-  <si>
-    <t>enpxdtwh</t>
-  </si>
-  <si>
-    <t>185.24.233.182:4009</t>
-  </si>
-  <si>
-    <t>Johnsson</t>
-  </si>
-  <si>
-    <t>frankinsonleejhonson5@gmail.com</t>
-  </si>
-  <si>
-    <t>vznrcpwb</t>
-  </si>
-  <si>
-    <t>mrshahimranshovon@gmail.com</t>
-  </si>
-  <si>
-    <t>twg5ZmvBqsixAfr</t>
-  </si>
-  <si>
-    <t>8GbKtEpRUr29jbg6</t>
-  </si>
-  <si>
-    <t>Shah</t>
-  </si>
-  <si>
-    <t>Imran</t>
+    <t>Elvis</t>
+  </si>
+  <si>
+    <t>Nolte</t>
+  </si>
+  <si>
+    <t>nolteelvis606@gmail.com</t>
+  </si>
+  <si>
+    <t>CHNFGJrturtiru4574</t>
+  </si>
+  <si>
+    <t>81.28.96.207:4021</t>
+  </si>
+  <si>
+    <t>PDmZ3WXF9RUC89KV</t>
+  </si>
+  <si>
+    <t>d8CUDDcpXHbgpgHh</t>
+  </si>
+  <si>
+    <t>Marie</t>
+  </si>
+  <si>
+    <t>Hughes</t>
+  </si>
+  <si>
+    <t>mariehughes053@gmail.com</t>
+  </si>
+  <si>
+    <t>yzhsybdywhud</t>
+  </si>
+  <si>
+    <t>81.28.96.212:4046</t>
+  </si>
+  <si>
+    <t>X7TAePrnpFSjx7XT</t>
+  </si>
+  <si>
+    <t>qZYMuNafMchx5nz4</t>
+  </si>
+  <si>
+    <t>Craig</t>
+  </si>
+  <si>
+    <t>Winstead</t>
+  </si>
+  <si>
+    <t>craig7winstead614455@gmail.com</t>
+  </si>
+  <si>
+    <t>Cvbn2582</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4005</t>
+  </si>
+  <si>
+    <t>pp3wCwtFw7r6GmwY</t>
+  </si>
+  <si>
+    <t>pbnXAK4KurcpTmEB</t>
+  </si>
+  <si>
+    <t>Joan</t>
+  </si>
+  <si>
+    <t>Turner</t>
+  </si>
+  <si>
+    <t>Joanturner45632@gmail.com</t>
+  </si>
+  <si>
+    <t>fwchspxmqa</t>
+  </si>
+  <si>
+    <t>81.28.96.212:4026</t>
+  </si>
+  <si>
+    <t>Alex</t>
+  </si>
+  <si>
+    <t>Romajun</t>
+  </si>
+  <si>
+    <t>romajunalex01890@gmail.com</t>
+  </si>
+  <si>
+    <t>XCVDFSreteryt4564</t>
+  </si>
+  <si>
+    <t>81.28.96.207:4025</t>
+  </si>
+  <si>
+    <t>Lisa</t>
+  </si>
+  <si>
+    <t>Hawkinse</t>
+  </si>
+  <si>
+    <t>hawkinselisa926@gmail.com</t>
+  </si>
+  <si>
+    <t>dpcjzhfbea</t>
+  </si>
+  <si>
+    <t>81.28.96.212:4038</t>
+  </si>
+  <si>
+    <t>Anibal</t>
+  </si>
+  <si>
+    <t>Lillard</t>
+  </si>
+  <si>
+    <t>aaniballlillard376@gmail.com</t>
+  </si>
+  <si>
+    <t>CDFfre34</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4002</t>
+  </si>
+  <si>
+    <t>Benjamin</t>
+  </si>
+  <si>
+    <t>Douthit</t>
+  </si>
+  <si>
+    <t>benjamindouthit555@gmail.com</t>
+  </si>
+  <si>
+    <t>AliVE108</t>
+  </si>
+  <si>
+    <t>192.227.142.207:3160</t>
+  </si>
+  <si>
+    <t>ffJXcZqmbUH8764W</t>
+  </si>
+  <si>
+    <t>QYcQAKBBr4REYqnp</t>
+  </si>
+  <si>
+    <t>Catherine</t>
+  </si>
+  <si>
+    <t>Bailey</t>
+  </si>
+  <si>
+    <t>cb48272@gmail.com</t>
+  </si>
+  <si>
+    <t>XDFJ&amp;^^%$#&amp;***(D456</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4016</t>
+  </si>
+  <si>
+    <t>Madison</t>
+  </si>
+  <si>
+    <t>Daniels</t>
+  </si>
+  <si>
+    <t>danielsmadison14@gmail.com</t>
+  </si>
+  <si>
+    <t>fxbsybxyshu</t>
+  </si>
+  <si>
+    <t>81.28.96.147:4020</t>
+  </si>
+  <si>
+    <t>3kJnrnp9pLc5eW64</t>
+  </si>
+  <si>
+    <t>55qcuaAF6KsJzYp8</t>
+  </si>
+  <si>
+    <t>Lorik</t>
+  </si>
+  <si>
+    <t>Frash毛ria</t>
+  </si>
+  <si>
+    <t>lorikfrasheria1@gmail.com</t>
+  </si>
+  <si>
+    <t>gRoYWXwxdJ</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4029</t>
+  </si>
+  <si>
+    <t>Ronald</t>
+  </si>
+  <si>
+    <t>Gibb</t>
+  </si>
+  <si>
+    <t>ronaldgibb778@gmail.com</t>
+  </si>
+  <si>
+    <t>gghh1122</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4027</t>
+  </si>
+  <si>
+    <t>Neca</t>
+  </si>
+  <si>
+    <t>Rivera</t>
+  </si>
+  <si>
+    <t>necarivera390@gmail.com</t>
+  </si>
+  <si>
+    <t>gxheyhdywhyd</t>
+  </si>
+  <si>
+    <t>81.28.96.147:4027</t>
+  </si>
+  <si>
+    <t>Carol</t>
+  </si>
+  <si>
+    <t>Howard</t>
+  </si>
+  <si>
+    <t>CarolHoward3262@gmail.com</t>
+  </si>
+  <si>
+    <t>How45ta34d</t>
+  </si>
+  <si>
+    <t>81.28.96.212:4040</t>
+  </si>
+  <si>
+    <t>Jean</t>
+  </si>
+  <si>
+    <t>Wilsone</t>
+  </si>
+  <si>
+    <t>wilsonejean66@gmail.com</t>
+  </si>
+  <si>
+    <t>xweuhcnzdk</t>
+  </si>
+  <si>
+    <t>81.28.96.134:45595</t>
+  </si>
+  <si>
+    <t>8ZWxTTnk5EG2JsYG</t>
+  </si>
+  <si>
+    <t>4MGK6SU9ySc66vJF</t>
+  </si>
+  <si>
+    <t>Orgest</t>
+  </si>
+  <si>
+    <t>Bogdanir</t>
+  </si>
+  <si>
+    <t>Autumncorataylerlop726@gmail.com</t>
+  </si>
+  <si>
+    <t>dcbalquuzr</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4007</t>
+  </si>
+  <si>
+    <t>Joe</t>
+  </si>
+  <si>
+    <t>Baidwn</t>
+  </si>
+  <si>
+    <t>joebaidwn1@gmail.com</t>
+  </si>
+  <si>
+    <t>CXBGDFHrtutryi678</t>
+  </si>
+  <si>
+    <t>81.28.96.207:4023</t>
+  </si>
+  <si>
+    <t>Mary</t>
+  </si>
+  <si>
+    <t>Fishera</t>
+  </si>
+  <si>
+    <t>maryfishera7@gmail.com</t>
+  </si>
+  <si>
+    <t>Kolomq1w2s</t>
+  </si>
+  <si>
+    <t>81.28.96.147:4014</t>
+  </si>
+  <si>
+    <t>Julie</t>
+  </si>
+  <si>
+    <t>Hasen</t>
+  </si>
+  <si>
+    <t>jhasen302@gmail.com</t>
+  </si>
+  <si>
+    <t>ZDFH()(*^%^$%@SDG56</t>
+  </si>
+  <si>
+    <t>Rosalind</t>
+  </si>
+  <si>
+    <t>Moreno</t>
+  </si>
+  <si>
+    <t>rosalindmoreno53875@gmail.com</t>
+  </si>
+  <si>
+    <t>FGJHG';\;[]=-0JKL57Y</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4023</t>
+  </si>
+  <si>
+    <t>Daren</t>
+  </si>
+  <si>
+    <t>Danis</t>
+  </si>
+  <si>
+    <t>darendanis221@gmail.com</t>
+  </si>
+  <si>
+    <t>PAINful00</t>
+  </si>
+  <si>
+    <t>81.28.96.212:4023</t>
+  </si>
+  <si>
+    <t>Courtney</t>
+  </si>
+  <si>
+    <t>Gowin</t>
+  </si>
+  <si>
+    <t>courtney2gowin6445@gmail.com</t>
+  </si>
+  <si>
+    <t>Derf9879</t>
+  </si>
+  <si>
+    <t>Keishlyann</t>
+  </si>
+  <si>
+    <t>Marcano</t>
+  </si>
+  <si>
+    <t>keishlyannm16@gmail.com</t>
+  </si>
+  <si>
+    <t>gzbsybxtehuf</t>
+  </si>
+  <si>
+    <t>81.28.96.147:4015</t>
+  </si>
+  <si>
+    <t>Tari</t>
+  </si>
+  <si>
+    <t>Gy枚ngyi</t>
+  </si>
+  <si>
+    <t>tarigyongyihu12@gmail.com</t>
+  </si>
+  <si>
+    <t>howareyouhu12</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4039</t>
+  </si>
+  <si>
+    <t>Margaret</t>
+  </si>
+  <si>
+    <t>Nelson</t>
+  </si>
+  <si>
+    <t>Margaretnelson56743@gmail.com</t>
+  </si>
+  <si>
+    <t>smeyfbukwd</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4047</t>
+  </si>
+  <si>
+    <t>Clark</t>
+  </si>
+  <si>
+    <t>Nion</t>
+  </si>
+  <si>
+    <t>clarknion861@gmail.com</t>
+  </si>
+  <si>
+    <t>gdhwyhfyhd</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4041</t>
+  </si>
+  <si>
+    <t>Sandra</t>
+  </si>
+  <si>
+    <t>Thiel</t>
+  </si>
+  <si>
+    <t>sandrathiel7638@gmail.com</t>
+  </si>
+  <si>
+    <t>FGJKGK\';\;[]-90H567G</t>
+  </si>
+  <si>
+    <t>Katherine</t>
+  </si>
+  <si>
+    <t>Dixon</t>
+  </si>
+  <si>
+    <t>isanjerin37579@gmail.com</t>
+  </si>
+  <si>
+    <t>XDZFGStyritiktri47474</t>
+  </si>
+  <si>
+    <t>81.28.96.207:4036</t>
+  </si>
+  <si>
+    <t>Moses</t>
+  </si>
+  <si>
+    <t>Synder</t>
+  </si>
+  <si>
+    <t>mosessynder334@gmail.com</t>
+  </si>
+  <si>
+    <t>Ftyhui90</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4024</t>
+  </si>
+  <si>
+    <t>Adam</t>
+  </si>
+  <si>
+    <t>Xampa</t>
+  </si>
+  <si>
+    <t>adamxampa733@gmail.com</t>
+  </si>
+  <si>
+    <t>CVBDFrtyutruifgh567</t>
+  </si>
+  <si>
+    <t>23.94.96.119:3139</t>
+  </si>
+  <si>
+    <t>6TFkNpfJJP2mVJ27</t>
+  </si>
+  <si>
+    <t>98hyShw5PC9D2vgw</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Wilham</t>
+  </si>
+  <si>
+    <t>wilhamdavid03@gmail.com</t>
+  </si>
+  <si>
+    <t>fchtysd573w4rgh</t>
+  </si>
+  <si>
+    <t>Julia</t>
+  </si>
+  <si>
+    <t>Peterse</t>
+  </si>
+  <si>
+    <t>juliapeterse78@gmail.com</t>
+  </si>
+  <si>
+    <t>zakbfjwqhs</t>
+  </si>
+  <si>
+    <t>81.28.96.212:4027</t>
+  </si>
+  <si>
+    <t>Alexis</t>
+  </si>
+  <si>
+    <t>Chapman</t>
+  </si>
+  <si>
+    <t>DamonSprains852@gmail.com</t>
+  </si>
+  <si>
+    <t>dsfvg2020</t>
+  </si>
+  <si>
+    <t>81.28.96.207:4020</t>
+  </si>
+  <si>
+    <t>Kemo</t>
+  </si>
+  <si>
+    <t>Paul</t>
+  </si>
+  <si>
+    <t>kemopaul8931@gmail.com</t>
+  </si>
+  <si>
+    <t>CBDFHtyrtfhryt4556</t>
+  </si>
+  <si>
+    <t>Olga</t>
+  </si>
+  <si>
+    <t>Mazur</t>
+  </si>
+  <si>
+    <t>olgamazurpo01@gmail.com</t>
+  </si>
+  <si>
+    <t>howareyoupo01</t>
+  </si>
+  <si>
+    <t>Louis</t>
+  </si>
+  <si>
+    <t>Longer</t>
+  </si>
+  <si>
+    <t>longerlouis029@gmail.com</t>
+  </si>
+  <si>
+    <t>ukzyfqjegv</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4015</t>
+  </si>
+  <si>
+    <t>alex</t>
+  </si>
+  <si>
+    <t>heals</t>
+  </si>
+  <si>
+    <t>Alexheal77@gmail.com</t>
+  </si>
+  <si>
+    <t>CXVBDFerteryg456</t>
+  </si>
+  <si>
+    <t>23.94.96.119:3134</t>
+  </si>
+  <si>
+    <t>Kathy</t>
+  </si>
+  <si>
+    <t>Crawford</t>
+  </si>
+  <si>
+    <t>kathycrawford284@gmail.com</t>
+  </si>
+  <si>
+    <t>XCBDF#$($#@!DFH454</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4008</t>
+  </si>
+  <si>
+    <t>Mitchell</t>
+  </si>
+  <si>
+    <t>Krupa</t>
+  </si>
+  <si>
+    <t>mitchellkrupa572@gmail.com</t>
+  </si>
+  <si>
+    <t>HEsitate18</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4035</t>
+  </si>
+  <si>
+    <t>Sanford</t>
+  </si>
+  <si>
+    <t>Eddington</t>
+  </si>
+  <si>
+    <t>sanfordeddington290@gmail.com</t>
+  </si>
+  <si>
+    <t>Jiuhygt68</t>
+  </si>
+  <si>
+    <t>Lamela</t>
+  </si>
+  <si>
+    <t>Sarabia</t>
+  </si>
+  <si>
+    <t>LamelaSarabia479n@gmail.com</t>
+  </si>
+  <si>
+    <t>maperhttre</t>
+  </si>
+  <si>
+    <t>81.28.96.212:4037</t>
+  </si>
+  <si>
+    <t>Rahano</t>
+  </si>
+  <si>
+    <t>joerahano36@gmail.com</t>
+  </si>
+  <si>
+    <t>CVBDFHrtyrtiur457</t>
+  </si>
+  <si>
+    <t>Shirley</t>
+  </si>
+  <si>
+    <t>Brinegar</t>
+  </si>
+  <si>
+    <t>shireyaberinegar546@gmail.com</t>
+  </si>
+  <si>
+    <t>GTFCkoiu36</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4030</t>
+  </si>
+  <si>
+    <t>Teresa</t>
+  </si>
+  <si>
+    <t>Scott</t>
+  </si>
+  <si>
+    <t>Teresascott78954@gmail.com</t>
+  </si>
+  <si>
+    <t>sdythjhwhtjnsdsd</t>
+  </si>
+  <si>
+    <t>81.28.96.147:4017</t>
+  </si>
+  <si>
+    <t>Noel</t>
+  </si>
+  <si>
+    <t>Demirir</t>
+  </si>
+  <si>
+    <t>noeldemirir86@gmail.com</t>
+  </si>
+  <si>
+    <t>M4hF09KH4K</t>
+  </si>
+  <si>
+    <t>81.28.96.212:4035</t>
+  </si>
+  <si>
+    <t>Michele</t>
+  </si>
+  <si>
+    <t>George</t>
+  </si>
+  <si>
+    <t>MicheleGeorge56354@gmail.com</t>
+  </si>
+  <si>
+    <t>Htarthjiqwdsds</t>
+  </si>
+  <si>
+    <t>23.94.96.119:3140</t>
+  </si>
+  <si>
+    <t>Rueben</t>
+  </si>
+  <si>
+    <t>Fannin</t>
+  </si>
+  <si>
+    <t>ruebenfannin777@gmail.com</t>
+  </si>
+  <si>
+    <t>Gasytui10</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4026</t>
+  </si>
+  <si>
+    <t>Kelly</t>
+  </si>
+  <si>
+    <t>Lawsone</t>
+  </si>
+  <si>
+    <t>kellylawsone5@gmail.com</t>
+  </si>
+  <si>
+    <t>sbzqmtfngv</t>
+  </si>
+  <si>
+    <t>Tiffany</t>
+  </si>
+  <si>
+    <t>Perkins</t>
+  </si>
+  <si>
+    <t>tp548710@gmail.com</t>
+  </si>
+  <si>
+    <t>CXFG@$@$^&amp;#%*454G</t>
+  </si>
+  <si>
+    <t>81.28.96.137:4009</t>
+  </si>
+  <si>
+    <t>Sherry</t>
+  </si>
+  <si>
+    <t>Romero</t>
+  </si>
+  <si>
+    <t>SherryRomero56534@gmail.com</t>
+  </si>
+  <si>
+    <t>Hd4tr5q3rASSEggd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -265,6 +940,18 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -447,7 +1134,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -562,6 +1249,21 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color rgb="FFCCCCCC"/>
+      </left>
+      <right style="medium">
+        <color rgb="FFCCCCCC"/>
+      </right>
+      <top style="medium">
+        <color rgb="FFCCCCCC"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FFCCCCCC"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -607,8 +1309,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1" readingOrder="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -930,177 +1636,1189 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="A2" sqref="A1:G51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="14.4" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="54" thickBot="1">
+      <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="54" thickBot="1">
+      <c r="A4" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="54" thickBot="1">
+      <c r="A5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="54" thickBot="1">
+      <c r="A6" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B6" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="C6" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G6" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
+    <row r="7" spans="1:7" ht="54" thickBot="1">
+      <c r="A7" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="54" thickBot="1">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="54" thickBot="1">
+      <c r="A9" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A10" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="54" thickBot="1">
+      <c r="A11" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A12" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A13" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A14" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="54" thickBot="1">
+      <c r="A15" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A16" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="54" thickBot="1">
+      <c r="A17" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A18" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G18" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B4" t="s">
-        <v>15</v>
-      </c>
-      <c r="C4" t="s">
-        <v>16</v>
-      </c>
-      <c r="D4" t="s">
-        <v>17</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
+    <row r="19" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A19" s="2" t="s">
+        <v>104</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>107</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>108</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A20" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>112</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="54" thickBot="1">
+      <c r="A21" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A22" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>120</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>121</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" ht="54" thickBot="1">
+      <c r="A23" s="2" t="s">
+        <v>123</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A24" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" ht="54" thickBot="1">
+      <c r="A25" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" ht="54" thickBot="1">
+      <c r="A26" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A27" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" ht="54" thickBot="1">
+      <c r="A28" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>117</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A29" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F29" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G4" t="s">
+      <c r="G29" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="30" spans="1:7" ht="54" thickBot="1">
+      <c r="A30" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>159</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A31" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A32" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A33" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="F33" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="C5" t="s">
+      <c r="G33" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" t="s">
+    </row>
+    <row r="34" spans="1:7" ht="54" thickBot="1">
+      <c r="A34" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="F34" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G5" t="s">
+      <c r="G34" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C6" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" t="s">
+    <row r="35" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A35" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A36" s="2" t="s">
+        <v>186</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>187</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>188</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>189</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G36" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A37" s="2" t="s">
+        <v>190</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>191</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>192</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A38" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="54" thickBot="1">
+      <c r="A39" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="54" thickBot="1">
+      <c r="A40" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="B40" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="C40" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E40" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="F40" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G40" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="54" thickBot="1">
+      <c r="A41" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="B41" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="C41" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D41" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="E41" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="F41" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G41" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="54" thickBot="1">
+      <c r="A42" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="B42" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="E42" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A43" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="B43" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>103</v>
+      </c>
+      <c r="F43" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G6" t="s">
+      <c r="G43" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="44" spans="1:7" ht="54" thickBot="1">
+      <c r="A44" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="B44" s="2" t="s">
+        <v>223</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>225</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>226</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G44" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="C7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D7" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
+    </row>
+    <row r="45" spans="1:7" ht="54" thickBot="1">
+      <c r="A45" s="2" t="s">
+        <v>227</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>228</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>229</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>230</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>231</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A46" s="2" t="s">
+        <v>232</v>
+      </c>
+      <c r="B46" s="2" t="s">
+        <v>233</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>234</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>236</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" ht="54" thickBot="1">
+      <c r="A47" s="2" t="s">
+        <v>237</v>
+      </c>
+      <c r="B47" s="2" t="s">
+        <v>238</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>240</v>
+      </c>
+      <c r="E47" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F47" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G47" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" ht="54" thickBot="1">
+      <c r="A48" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="B48" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="F48" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G48" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A49" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B49" s="2" t="s">
+        <v>248</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>249</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>250</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F49" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="G49" s="2" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" ht="40.799999999999997" thickBot="1">
+      <c r="A50" s="2" t="s">
+        <v>251</v>
+      </c>
+      <c r="B50" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C50" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D50" s="2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="F50" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G50" s="2" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" ht="54" thickBot="1">
+      <c r="A51" s="2" t="s">
+        <v>256</v>
+      </c>
+      <c r="B51" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C51" s="2" t="s">
+        <v>258</v>
+      </c>
+      <c r="D51" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>241</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="G51" s="2" t="s">
+        <v>167</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
saving related problem fixed
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -94,13 +94,34 @@
   </si>
   <si>
     <t>&amp;lCLm&amp;yU</t>
+  </si>
+  <si>
+    <t>lorettabowers06@gmail.com</t>
+  </si>
+  <si>
+    <t>Oruyr1TRgsErtMb</t>
+  </si>
+  <si>
+    <t>81.28.96.125:18156</t>
+  </si>
+  <si>
+    <t>g72j7SmGDfQ6DsmZ</t>
+  </si>
+  <si>
+    <t>2HaMyW78WzQb224X</t>
+  </si>
+  <si>
+    <t>Bowers</t>
+  </si>
+  <si>
+    <t>Loretta</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -240,6 +261,11 @@
       <color indexed="8"/>
       <name val="Arial"/>
       <charset val="134"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -598,11 +624,12 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -927,11 +954,13 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K11" sqref="K11"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
+    <col min="2" max="2" width="12.44140625" customWidth="1"/>
+    <col min="3" max="3" width="20.88671875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
@@ -1005,7 +1034,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="15" thickBot="1">
+    <row r="4" spans="1:7">
       <c r="A4" t="s">
         <v>21</v>
       </c>
@@ -1029,13 +1058,27 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1">
-      <c r="A5" s="1"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
-      <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
-      <c r="G5" s="1"/>
+      <c r="A5" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="C5" t="s">
+        <v>25</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1">
       <c r="A6" s="1"/>
@@ -1444,5 +1487,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
done till sending the mail
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\2020\gmail_app\gmail_app_old\gmail_app\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="group_a" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0" iterateDelta="1E-4"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -63,58 +63,25 @@
     <t>gV9XKZj2J47VwkeY</t>
   </si>
   <si>
-    <t>Elnora</t>
-  </si>
-  <si>
-    <t>Schmitt</t>
-  </si>
-  <si>
-    <t>elnoraschmitt426@gmail.com</t>
-  </si>
-  <si>
-    <t>&amp;m2&amp;&amp;maW</t>
-  </si>
-  <si>
-    <t>23.154.81.120:38986</t>
-  </si>
-  <si>
-    <t>y7qVkXbykT7wUEH6</t>
-  </si>
-  <si>
-    <t>fAdts4NQZ9EsC5wj</t>
-  </si>
-  <si>
-    <t>Toshiko</t>
-  </si>
-  <si>
-    <t>Monahan</t>
-  </si>
-  <si>
-    <t>monahantoshiko226@gmail.com</t>
-  </si>
-  <si>
-    <t>&amp;lCLm&amp;yU</t>
-  </si>
-  <si>
-    <t>lorettabowers06@gmail.com</t>
-  </si>
-  <si>
-    <t>Oruyr1TRgsErtMb</t>
-  </si>
-  <si>
-    <t>81.28.96.125:18156</t>
-  </si>
-  <si>
-    <t>g72j7SmGDfQ6DsmZ</t>
-  </si>
-  <si>
-    <t>2HaMyW78WzQb224X</t>
-  </si>
-  <si>
-    <t>Bowers</t>
-  </si>
-  <si>
-    <t>Loretta</t>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Gibbons</t>
+  </si>
+  <si>
+    <t>0101dave.gibbons22@gmail.com</t>
+  </si>
+  <si>
+    <t>wlmgbnezgtgglefg</t>
+  </si>
+  <si>
+    <t>81.28.96.131:58065</t>
+  </si>
+  <si>
+    <t>Ks4BcUQh43z8AjTF</t>
+  </si>
+  <si>
+    <t>E44dyaN4k3F3MPkH</t>
   </si>
 </sst>
 </file>
@@ -257,15 +224,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <sz val="9"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="33">
@@ -626,10 +594,10 @@
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment wrapText="1" readingOrder="1"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -951,542 +919,520 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G50"/>
+  <dimension ref="A1:G51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A2" sqref="A1:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="12.44140625" customWidth="1"/>
-    <col min="3" max="3" width="20.88671875" customWidth="1"/>
     <col min="5" max="5" width="25" customWidth="1"/>
     <col min="6" max="6" width="32.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="14.4" customHeight="1">
-      <c r="A1" t="s">
+    <row r="1" spans="1:7" ht="14.4" customHeight="1" thickBot="1">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+    <row r="2" spans="1:7" ht="15" thickBot="1">
+      <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="F2" t="s">
+      <c r="F2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="G2" t="s">
+      <c r="G2" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" ht="15" thickBot="1">
+      <c r="A3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G3" t="s">
+      <c r="G3" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-      <c r="E4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G4" t="s">
-        <v>20</v>
-      </c>
+    <row r="4" spans="1:7" ht="15" thickBot="1">
+      <c r="A4" s="2"/>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
+      <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15" thickBot="1">
-      <c r="A5" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="C5" t="s">
-        <v>25</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="G5" s="2" t="s">
-        <v>29</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
+      <c r="E5" s="2"/>
+      <c r="F5" s="2"/>
+      <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15" thickBot="1">
-      <c r="A6" s="1"/>
-      <c r="B6" s="1"/>
-      <c r="C6" s="1"/>
-      <c r="D6" s="1"/>
-      <c r="E6" s="1"/>
-      <c r="F6" s="1"/>
-      <c r="G6" s="1"/>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
+      <c r="C6" s="2"/>
+      <c r="D6" s="2"/>
+      <c r="E6" s="2"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15" thickBot="1">
-      <c r="A7" s="1"/>
-      <c r="B7" s="1"/>
-      <c r="C7" s="1"/>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
-      <c r="G7" s="1"/>
+      <c r="A7" s="2"/>
+      <c r="B7" s="2"/>
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1">
-      <c r="A8" s="1"/>
-      <c r="B8" s="1"/>
-      <c r="C8" s="1"/>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1"/>
-      <c r="F8" s="1"/>
-      <c r="G8" s="1"/>
+      <c r="A8" s="2"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="15" thickBot="1">
-      <c r="A9" s="1"/>
-      <c r="B9" s="1"/>
-      <c r="C9" s="1"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
+      <c r="A9" s="2"/>
+      <c r="B9" s="2"/>
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7" ht="15" thickBot="1">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1"/>
-      <c r="C10" s="1"/>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1"/>
-      <c r="F10" s="1"/>
-      <c r="G10" s="1"/>
+      <c r="A10" s="2"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+      <c r="E10" s="2"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7" ht="15" thickBot="1">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1"/>
-      <c r="C11" s="1"/>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1"/>
-      <c r="F11" s="1"/>
-      <c r="G11" s="1"/>
+      <c r="A11" s="2"/>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="2"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
     </row>
     <row r="12" spans="1:7" ht="15" thickBot="1">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
+      <c r="A12" s="2"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
     </row>
     <row r="13" spans="1:7" ht="15" thickBot="1">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
+      <c r="A13" s="2"/>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
     </row>
     <row r="14" spans="1:7" ht="15" thickBot="1">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
-      <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="1"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
+      <c r="A14" s="2"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
+      <c r="A15" s="2"/>
+      <c r="B15" s="2"/>
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="15" thickBot="1">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
+      <c r="A16" s="2"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
     </row>
     <row r="17" spans="1:7" ht="15" thickBot="1">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="1"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
+      <c r="A17" s="2"/>
+      <c r="B17" s="2"/>
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
     </row>
     <row r="18" spans="1:7" ht="15" thickBot="1">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="1"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
+      <c r="A18" s="2"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
     </row>
     <row r="19" spans="1:7" ht="15" thickBot="1">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="1"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
+      <c r="A19" s="2"/>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
     </row>
     <row r="20" spans="1:7" ht="15" thickBot="1">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="1"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
+      <c r="A20" s="2"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="2"/>
+      <c r="D20" s="2"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
     </row>
     <row r="21" spans="1:7" ht="15" thickBot="1">
-      <c r="A21" s="1"/>
-      <c r="B21" s="1"/>
-      <c r="C21" s="1"/>
-      <c r="D21" s="1"/>
-      <c r="E21" s="1"/>
-      <c r="F21" s="1"/>
-      <c r="G21" s="1"/>
+      <c r="A21" s="2"/>
+      <c r="B21" s="2"/>
+      <c r="C21" s="2"/>
+      <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:7" ht="15" thickBot="1">
-      <c r="A22" s="1"/>
-      <c r="B22" s="1"/>
-      <c r="C22" s="1"/>
-      <c r="D22" s="1"/>
-      <c r="E22" s="1"/>
-      <c r="F22" s="1"/>
-      <c r="G22" s="1"/>
+      <c r="A22" s="2"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="2"/>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
+      <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:7" ht="15" thickBot="1">
-      <c r="A23" s="1"/>
-      <c r="B23" s="1"/>
-      <c r="C23" s="1"/>
-      <c r="D23" s="1"/>
-      <c r="E23" s="1"/>
-      <c r="F23" s="1"/>
-      <c r="G23" s="1"/>
+      <c r="A23" s="2"/>
+      <c r="B23" s="2"/>
+      <c r="C23" s="2"/>
+      <c r="D23" s="2"/>
+      <c r="E23" s="2"/>
+      <c r="F23" s="2"/>
+      <c r="G23" s="2"/>
     </row>
     <row r="24" spans="1:7" ht="15" thickBot="1">
-      <c r="A24" s="1"/>
-      <c r="B24" s="1"/>
-      <c r="C24" s="1"/>
-      <c r="D24" s="1"/>
-      <c r="E24" s="1"/>
-      <c r="F24" s="1"/>
-      <c r="G24" s="1"/>
+      <c r="A24" s="2"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+      <c r="D24" s="2"/>
+      <c r="E24" s="2"/>
+      <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:7" ht="15" thickBot="1">
-      <c r="A25" s="1"/>
-      <c r="B25" s="1"/>
-      <c r="C25" s="1"/>
-      <c r="D25" s="1"/>
-      <c r="E25" s="1"/>
-      <c r="F25" s="1"/>
-      <c r="G25" s="1"/>
+      <c r="A25" s="2"/>
+      <c r="B25" s="2"/>
+      <c r="C25" s="2"/>
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:7" ht="15" thickBot="1">
-      <c r="A26" s="1"/>
-      <c r="B26" s="1"/>
-      <c r="C26" s="1"/>
-      <c r="D26" s="1"/>
-      <c r="E26" s="1"/>
-      <c r="F26" s="1"/>
-      <c r="G26" s="1"/>
+      <c r="A26" s="2"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2"/>
+      <c r="E26" s="2"/>
+      <c r="F26" s="2"/>
+      <c r="G26" s="2"/>
     </row>
     <row r="27" spans="1:7" ht="15" thickBot="1">
-      <c r="A27" s="1"/>
-      <c r="B27" s="1"/>
-      <c r="C27" s="1"/>
-      <c r="D27" s="1"/>
-      <c r="E27" s="1"/>
-      <c r="F27" s="1"/>
-      <c r="G27" s="1"/>
+      <c r="A27" s="2"/>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" s="2"/>
+      <c r="G27" s="2"/>
     </row>
     <row r="28" spans="1:7" ht="15" thickBot="1">
-      <c r="A28" s="1"/>
-      <c r="B28" s="1"/>
-      <c r="C28" s="1"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:7" ht="15" thickBot="1">
-      <c r="A29" s="1"/>
-      <c r="B29" s="1"/>
-      <c r="C29" s="1"/>
-      <c r="D29" s="1"/>
-      <c r="E29" s="1"/>
-      <c r="F29" s="1"/>
-      <c r="G29" s="1"/>
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+      <c r="G29" s="2"/>
     </row>
     <row r="30" spans="1:7" ht="15" thickBot="1">
-      <c r="A30" s="1"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="1"/>
-      <c r="D30" s="1"/>
-      <c r="E30" s="1"/>
-      <c r="F30" s="1"/>
-      <c r="G30" s="1"/>
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:7" ht="15" thickBot="1">
-      <c r="A31" s="1"/>
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-      <c r="D31" s="1"/>
-      <c r="E31" s="1"/>
-      <c r="F31" s="1"/>
-      <c r="G31" s="1"/>
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+      <c r="G31" s="2"/>
     </row>
     <row r="32" spans="1:7" ht="15" thickBot="1">
-      <c r="A32" s="1"/>
-      <c r="B32" s="1"/>
-      <c r="C32" s="1"/>
-      <c r="D32" s="1"/>
-      <c r="E32" s="1"/>
-      <c r="F32" s="1"/>
-      <c r="G32" s="1"/>
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+      <c r="G32" s="2"/>
     </row>
     <row r="33" spans="1:7" ht="15" thickBot="1">
-      <c r="A33" s="1"/>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-      <c r="D33" s="1"/>
-      <c r="E33" s="1"/>
-      <c r="F33" s="1"/>
-      <c r="G33" s="1"/>
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+      <c r="G33" s="2"/>
     </row>
     <row r="34" spans="1:7" ht="15" thickBot="1">
-      <c r="A34" s="1"/>
-      <c r="B34" s="1"/>
-      <c r="C34" s="1"/>
-      <c r="D34" s="1"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+      <c r="G34" s="2"/>
     </row>
     <row r="35" spans="1:7" ht="15" thickBot="1">
-      <c r="A35" s="1"/>
-      <c r="B35" s="1"/>
-      <c r="C35" s="1"/>
-      <c r="D35" s="1"/>
-      <c r="E35" s="1"/>
-      <c r="F35" s="1"/>
-      <c r="G35" s="1"/>
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
     </row>
     <row r="36" spans="1:7" ht="15" thickBot="1">
-      <c r="A36" s="1"/>
-      <c r="B36" s="1"/>
-      <c r="C36" s="1"/>
-      <c r="D36" s="1"/>
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
     </row>
     <row r="37" spans="1:7" ht="15" thickBot="1">
-      <c r="A37" s="1"/>
-      <c r="B37" s="1"/>
-      <c r="C37" s="1"/>
-      <c r="D37" s="1"/>
-      <c r="E37" s="1"/>
-      <c r="F37" s="1"/>
-      <c r="G37" s="1"/>
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+      <c r="G37" s="2"/>
     </row>
     <row r="38" spans="1:7" ht="15" thickBot="1">
-      <c r="A38" s="1"/>
-      <c r="B38" s="1"/>
-      <c r="C38" s="1"/>
-      <c r="D38" s="1"/>
-      <c r="E38" s="1"/>
-      <c r="F38" s="1"/>
-      <c r="G38" s="1"/>
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+      <c r="G38" s="2"/>
     </row>
     <row r="39" spans="1:7" ht="15" thickBot="1">
-      <c r="A39" s="1"/>
-      <c r="B39" s="1"/>
-      <c r="C39" s="1"/>
-      <c r="D39" s="1"/>
-      <c r="E39" s="1"/>
-      <c r="F39" s="1"/>
-      <c r="G39" s="1"/>
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
     </row>
     <row r="40" spans="1:7" ht="15" thickBot="1">
-      <c r="A40" s="1"/>
-      <c r="B40" s="1"/>
-      <c r="C40" s="1"/>
-      <c r="D40" s="1"/>
-      <c r="E40" s="1"/>
-      <c r="F40" s="1"/>
-      <c r="G40" s="1"/>
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
     </row>
     <row r="41" spans="1:7" ht="15" thickBot="1">
-      <c r="A41" s="1"/>
-      <c r="B41" s="1"/>
-      <c r="C41" s="1"/>
-      <c r="D41" s="1"/>
-      <c r="E41" s="1"/>
-      <c r="F41" s="1"/>
-      <c r="G41" s="1"/>
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+      <c r="G41" s="2"/>
     </row>
     <row r="42" spans="1:7" ht="15" thickBot="1">
-      <c r="A42" s="1"/>
-      <c r="B42" s="1"/>
-      <c r="C42" s="1"/>
-      <c r="D42" s="1"/>
-      <c r="E42" s="1"/>
-      <c r="F42" s="1"/>
-      <c r="G42" s="1"/>
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+      <c r="G42" s="2"/>
     </row>
     <row r="43" spans="1:7" ht="15" thickBot="1">
-      <c r="A43" s="1"/>
-      <c r="B43" s="1"/>
-      <c r="C43" s="1"/>
-      <c r="D43" s="1"/>
-      <c r="E43" s="1"/>
-      <c r="F43" s="1"/>
-      <c r="G43" s="1"/>
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
     </row>
     <row r="44" spans="1:7" ht="15" thickBot="1">
-      <c r="A44" s="1"/>
-      <c r="B44" s="1"/>
-      <c r="C44" s="1"/>
-      <c r="D44" s="1"/>
-      <c r="E44" s="1"/>
-      <c r="F44" s="1"/>
-      <c r="G44" s="1"/>
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+      <c r="G44" s="2"/>
     </row>
     <row r="45" spans="1:7" ht="15" thickBot="1">
-      <c r="A45" s="1"/>
-      <c r="B45" s="1"/>
-      <c r="C45" s="1"/>
-      <c r="D45" s="1"/>
-      <c r="E45" s="1"/>
-      <c r="F45" s="1"/>
-      <c r="G45" s="1"/>
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+      <c r="G45" s="2"/>
     </row>
     <row r="46" spans="1:7" ht="15" thickBot="1">
-      <c r="A46" s="1"/>
-      <c r="B46" s="1"/>
-      <c r="C46" s="1"/>
-      <c r="D46" s="1"/>
-      <c r="E46" s="1"/>
-      <c r="F46" s="1"/>
-      <c r="G46" s="1"/>
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+      <c r="G46" s="2"/>
     </row>
     <row r="47" spans="1:7" ht="15" thickBot="1">
-      <c r="A47" s="1"/>
-      <c r="B47" s="1"/>
-      <c r="C47" s="1"/>
-      <c r="D47" s="1"/>
-      <c r="E47" s="1"/>
-      <c r="F47" s="1"/>
-      <c r="G47" s="1"/>
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+      <c r="G47" s="2"/>
     </row>
     <row r="48" spans="1:7" ht="15" thickBot="1">
-      <c r="A48" s="1"/>
-      <c r="B48" s="1"/>
-      <c r="C48" s="1"/>
-      <c r="D48" s="1"/>
-      <c r="E48" s="1"/>
-      <c r="F48" s="1"/>
-      <c r="G48" s="1"/>
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+      <c r="G48" s="2"/>
     </row>
     <row r="49" spans="1:7" ht="15" thickBot="1">
-      <c r="A49" s="1"/>
-      <c r="B49" s="1"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="1"/>
-      <c r="E49" s="1"/>
-      <c r="F49" s="1"/>
-      <c r="G49" s="1"/>
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+      <c r="G49" s="2"/>
     </row>
     <row r="50" spans="1:7" ht="15" thickBot="1">
-      <c r="A50" s="1"/>
-      <c r="B50" s="1"/>
-      <c r="C50" s="1"/>
-      <c r="D50" s="1"/>
-      <c r="E50" s="1"/>
-      <c r="F50" s="1"/>
-      <c r="G50" s="1"/>
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+      <c r="G50" s="2"/>
+    </row>
+    <row r="51" spans="1:7" ht="15" thickBot="1">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+      <c r="G51" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
follow up smtp no uses json to store data on db
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="355">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="360">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -42,39 +42,12 @@
     <t>PROXY_PASS</t>
   </si>
   <si>
-    <t>Catrice</t>
-  </si>
-  <si>
-    <t>Kimball</t>
-  </si>
-  <si>
-    <t>catricekimball351@gmail.com</t>
-  </si>
-  <si>
-    <t>juodkinerrugvgfc</t>
-  </si>
-  <si>
-    <t>81.28.96.145:4001</t>
-  </si>
-  <si>
     <t>KpbXsNM7RkxsXfWr</t>
   </si>
   <si>
     <t>JYTtYbv6hPvJSqZc</t>
   </si>
   <si>
-    <t>Xuan</t>
-  </si>
-  <si>
-    <t>Warren</t>
-  </si>
-  <si>
-    <t>warrenxuan@gmail.com</t>
-  </si>
-  <si>
-    <t>lepmstwrprnzqdzi</t>
-  </si>
-  <si>
     <t>81.28.96.80:4007</t>
   </si>
   <si>
@@ -1084,6 +1057,48 @@
   </si>
   <si>
     <t>soyhhpendklfukwu</t>
+  </si>
+  <si>
+    <t>James</t>
+  </si>
+  <si>
+    <t>Calloway</t>
+  </si>
+  <si>
+    <t>jamescalloway402@gmail.com</t>
+  </si>
+  <si>
+    <t>whiqufiogheqkdvw</t>
+  </si>
+  <si>
+    <t>185.14.97.29:4001</t>
+  </si>
+  <si>
+    <t>eVLjgYYsF64zW8Zx</t>
+  </si>
+  <si>
+    <t>gV9XKZj2J47VwkeY</t>
+  </si>
+  <si>
+    <t>David</t>
+  </si>
+  <si>
+    <t>Gibbons</t>
+  </si>
+  <si>
+    <t>0101dave.gibbons22@gmail.com</t>
+  </si>
+  <si>
+    <t>wlmgbnezgtgglefg</t>
+  </si>
+  <si>
+    <t>81.28.96.131:58065</t>
+  </si>
+  <si>
+    <t>Ks4BcUQh43z8AjTF</t>
+  </si>
+  <si>
+    <t>E44dyaN4k3F3MPkH</t>
   </si>
 </sst>
 </file>
@@ -1893,7 +1908,7 @@
   <dimension ref="A1:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A1:XFD1048576"/>
+      <selection activeCell="N24" sqref="N24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1923,1635 +1938,1635 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>346</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>347</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>348</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>349</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>350</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>351</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>352</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>353</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>354</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>355</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>356</v>
       </c>
       <c r="E3" t="s">
-        <v>18</v>
+        <v>357</v>
       </c>
       <c r="F3" t="s">
-        <v>19</v>
+        <v>358</v>
       </c>
       <c r="G3" t="s">
-        <v>20</v>
+        <v>359</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>13</v>
       </c>
       <c r="C4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="D4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="E4" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
       <c r="F4" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="E5" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F5" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="B6" t="s">
-        <v>36</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="D6" t="s">
-        <v>38</v>
+        <v>29</v>
       </c>
       <c r="E6" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F6" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="B7" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="C7" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="D7" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="E7" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="C8" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="D8" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
       <c r="E8" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>53</v>
+        <v>44</v>
       </c>
       <c r="C9" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="D9" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="E9" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G9" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="B10" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="C10" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="D10" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="E10" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="F10" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G10" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B11" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C11" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="D11" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E11" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F11" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G11" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B12" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="E12" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F12" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G12" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B13" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="C13" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="D13" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="E13" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F13" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G13" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="B14" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="C14" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="D14" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="E14" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F14" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G14" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B15" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="D15" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="E15" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="F15" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G15" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="B16" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="C16" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="D16" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="E16" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="F16" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="G16" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="B17" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C17" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D17" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="E17" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F17" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G17" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="D18" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="E18" t="s">
-        <v>18</v>
+        <v>9</v>
       </c>
       <c r="F18" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B19" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C19" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="D19" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="E19" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F19" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G19" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B20" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C20" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="D20" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="E20" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F20" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G20" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B21" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C21" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="D21" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="E21" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F21" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G21" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="B22" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C22" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="D22" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="E22" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F22" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G22" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B23" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C23" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="D23" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="E23" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F23" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G23" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="B24" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="C24" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="D24" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="E24" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F24" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G24" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="C25" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="D25" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="E25" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F25" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G25" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B26" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C26" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="D26" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="E26" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F26" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G26" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B27" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C27" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="D27" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="E27" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F27" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G27" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B28" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C28" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="D28" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="E28" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F28" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G28" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B29" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C29" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="D29" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="E29" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F29" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G29" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B30" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C30" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="D30" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="E30" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="F30" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="G30" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C31" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="D31" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="E31" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F31" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G31" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="B32" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="C32" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="D32" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="E32" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F32" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G32" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B33" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C33" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="D33" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="E33" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="F33" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G33" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B34" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C34" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="D34" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="E34" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F34" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G34" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="B35" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="C35" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="D35" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="E35" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="F35" t="s">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="G35" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="B36" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="C36" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="D36" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="E36" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F36" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G36" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="B37" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="C37" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="D37" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="E37" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="F37" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="G37" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B38" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C38" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="D38" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="E38" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="F38" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G38" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B39" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C39" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="D39" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E39" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F39" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G39" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B40" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C40" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D40" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="E40" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F40" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G40" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B41" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C41" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="D41" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="E41" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F41" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="G41" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="B42" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="C42" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D42" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="E42" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F42" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="G42" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B43" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="C43" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="D43" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="E43" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="F43" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G43" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B44" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="C44" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="D44" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="E44" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F44" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G44" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="B45" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
       <c r="C45" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="D45" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
       <c r="E45" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
       <c r="F45" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G45" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
       <c r="B46" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C46" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
       <c r="D46" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
       <c r="E46" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
       <c r="F46" t="s">
-        <v>26</v>
+        <v>17</v>
       </c>
       <c r="G46" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
       <c r="B47" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
       <c r="C47" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
       <c r="D47" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
       <c r="E47" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F47" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G47" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
       <c r="B48" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
       <c r="C48" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
       <c r="D48" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="E48" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="F48" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G48" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
       <c r="B49" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
       <c r="C49" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
       <c r="D49" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
       <c r="E49" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="F49" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G49" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
       <c r="B50" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="C50" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
       <c r="D50" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
       <c r="E50" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F50" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G50" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
       <c r="B51" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
       <c r="C51" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
       <c r="D51" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
       <c r="E51" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
       <c r="F51" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G51" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
       <c r="B52" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
       <c r="C52" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
       <c r="D52" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
       <c r="E52" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F52" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G52" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
       <c r="B53" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
       <c r="C53" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="D53" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
       <c r="E53" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="F53" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="G53" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
       <c r="B54" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="C54" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
       <c r="D54" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
       <c r="E54" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="F54" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G54" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
       <c r="B55" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
       <c r="C55" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
       <c r="D55" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
       <c r="E55" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="F55" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G55" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
       <c r="B56" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
       <c r="C56" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
       <c r="D56" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
       <c r="E56" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F56" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="G56" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
       <c r="B57" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
       <c r="C57" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
       <c r="D57" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
       <c r="E57" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
       <c r="F57" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G57" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
       <c r="B58" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
       <c r="C58" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
       <c r="D58" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
       <c r="E58" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F58" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G58" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
       <c r="B59" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
       <c r="C59" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
       <c r="D59" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
       <c r="E59" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F59" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G59" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
       <c r="B60" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
       <c r="C60" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
       <c r="D60" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
       <c r="E60" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
       <c r="F60" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G60" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
       <c r="B61" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
       <c r="C61" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
       <c r="D61" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
       <c r="E61" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
       <c r="F61" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="G61" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
       <c r="B62" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
       <c r="C62" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
       <c r="D62" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
       <c r="E62" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="F62" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G62" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
       <c r="B63" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
       <c r="C63" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
       <c r="D63" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="E63" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="F63" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G63" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B64" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="C64" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
       <c r="D64" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="E64" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="F64" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G64" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="B65" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C65" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
       <c r="D65" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="E65" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="F65" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G65" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
       <c r="B66" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="C66" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="D66" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="E66" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="F66" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="G66" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B67" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="C67" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="D67" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
       <c r="E67" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="F67" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="G67" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="B68" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="C68" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
       <c r="D68" t="s">
-        <v>337</v>
+        <v>328</v>
       </c>
       <c r="E68" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="F68" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G68" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>338</v>
+        <v>329</v>
       </c>
       <c r="B69" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="C69" t="s">
-        <v>340</v>
+        <v>331</v>
       </c>
       <c r="D69" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
       <c r="E69" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="F69" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="G69" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B70" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="C70" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="D70" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="E70" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
       <c r="F70" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="G70" t="s">
-        <v>34</v>
+        <v>25</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
       <c r="B71" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="C71" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="D71" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="E71" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F71" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="G71" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
       <c r="B72" t="s">
-        <v>352</v>
+        <v>343</v>
       </c>
       <c r="C72" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D72" t="s">
-        <v>354</v>
+        <v>345</v>
       </c>
       <c r="E72" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="F72" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="G72" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
auto fire responses webhook
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -73,42 +73,6 @@
   </si>
   <si>
     <t>wrddcsqmfqdkqkrx</t>
-  </si>
-  <si>
-    <t>Jesus</t>
-  </si>
-  <si>
-    <t>Gaither</t>
-  </si>
-  <si>
-    <t>seyiowolabi487@gmail.com</t>
-  </si>
-  <si>
-    <t>ssgyqwzufpmmeauu</t>
-  </si>
-  <si>
-    <t>Russell</t>
-  </si>
-  <si>
-    <t>Wong</t>
-  </si>
-  <si>
-    <t>zhalilu1992@gmail.com</t>
-  </si>
-  <si>
-    <t>tdogxhumqufbpodh</t>
-  </si>
-  <si>
-    <t>Judy</t>
-  </si>
-  <si>
-    <t>Marvin</t>
-  </si>
-  <si>
-    <t>clementidakpo@gmail.com</t>
-  </si>
-  <si>
-    <t>fftanaopilfsqyog</t>
   </si>
 </sst>
 </file>
@@ -915,10 +879,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G6"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,75 +961,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="G4" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" t="s">
-        <v>23</v>
-      </c>
-      <c r="C5" t="s">
-        <v>24</v>
-      </c>
-      <c r="D5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" t="s">
-        <v>27</v>
-      </c>
-      <c r="C6" t="s">
-        <v>28</v>
-      </c>
-      <c r="D6" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
number of emails randomization
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34200" windowHeight="11616"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34200" windowHeight="11610"/>
   </bookViews>
   <sheets>
     <sheet name="group_a" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -42,27 +42,6 @@
     <t>PROXY_PASS</t>
   </si>
   <si>
-    <t>Louise</t>
-  </si>
-  <si>
-    <t>Deforge</t>
-  </si>
-  <si>
-    <t>saidunuhu579@gmail.com</t>
-  </si>
-  <si>
-    <t>ujemlxfzbgwnkzpd</t>
-  </si>
-  <si>
-    <t>185.125.171.221:4021</t>
-  </si>
-  <si>
-    <t>2JjU2izT4rk1tGb</t>
-  </si>
-  <si>
-    <t>bEjmSK36Ma4C36t</t>
-  </si>
-  <si>
     <t>Janice</t>
   </si>
   <si>
@@ -73,6 +52,15 @@
   </si>
   <si>
     <t>wrddcsqmfqdkqkrx</t>
+  </si>
+  <si>
+    <t>198.140.141.18:47299</t>
+  </si>
+  <si>
+    <t>xL50iQ642EZkOn</t>
+  </si>
+  <si>
+    <t>i8IhO2946aEDpf</t>
   </si>
 </sst>
 </file>
@@ -879,20 +867,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G3"/>
+  <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="G3" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="23.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -915,7 +903,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -935,29 +923,6 @@
         <v>12</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" t="s">
-        <v>17</v>
-      </c>
-      <c r="E3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" t="s">
-        <v>12</v>
-      </c>
-      <c r="G3" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>

<commit_message>
host randomization, unicode space and smtp proxy class changed
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -81,35 +81,17 @@
     <t>Whateverpass0*</t>
   </si>
   <si>
-    <t>davidgreenberg200@yahoo.com</t>
-  </si>
-  <si>
-    <t>David</t>
-  </si>
-  <si>
-    <t>Greenberg</t>
-  </si>
-  <si>
     <t>John</t>
   </si>
   <si>
     <t>Snow</t>
-  </si>
-  <si>
-    <t>wjagnkpeldenlxmq</t>
-  </si>
-  <si>
-    <t>davidgreenberg329@aol.com</t>
-  </si>
-  <si>
-    <t>david.greenberg23@zohomail.eu</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -246,23 +228,9 @@
     </font>
     <font>
       <sz val="10"/>
-      <color rgb="FF727479"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <color rgb="FFA9B7C6"/>
       <name val="Arial Unicode MS"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="33">
@@ -562,7 +530,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="43">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -605,19 +573,14 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="42" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="43">
+  <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -651,7 +614,6 @@
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="42" builtinId="8"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
     <cellStyle name="Neutral" xfId="8" builtinId="28" customBuiltin="1"/>
@@ -938,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I22" sqref="I22"/>
+      <selection activeCell="H22" sqref="H22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -978,16 +940,16 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>8</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="E2" t="s">
         <v>11</v>
@@ -1001,16 +963,16 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>14</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="C3" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>17</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>11</v>
@@ -1024,16 +986,16 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>23</v>
+        <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E4" t="s">
         <v>11</v>
@@ -1045,80 +1007,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E5" t="s">
-        <v>11</v>
-      </c>
-      <c r="F5" t="s">
-        <v>12</v>
-      </c>
-      <c r="G5" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>21</v>
-      </c>
-      <c r="B6" t="s">
-        <v>22</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="D6" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" t="s">
-        <v>12</v>
-      </c>
-      <c r="G6" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="15" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="D7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="E7" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" t="s">
-        <v>12</v>
-      </c>
-      <c r="G7" t="s">
-        <v>13</v>
-      </c>
+    <row r="5" spans="1:7" ht="15" x14ac:dyDescent="0.3">
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
moved to a new machine
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -85,6 +85,15 @@
   </si>
   <si>
     <t>Snow</t>
+  </si>
+  <si>
+    <t>81.28.96.148:4000</t>
+  </si>
+  <si>
+    <t>i0BdGW79w6Oo</t>
+  </si>
+  <si>
+    <t>5Ao37R1ry6bc</t>
   </si>
 </sst>
 </file>
@@ -903,7 +912,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H22" sqref="H22"/>
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -952,13 +961,13 @@
         <v>19</v>
       </c>
       <c r="E2" t="s">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="F2" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="G2" t="s">
-        <v>13</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
reply mail html foramttin related problem fixed
</commit_message>
<xml_diff>
--- a/database/group_a.xlsx
+++ b/database/group_a.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27830"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Upwork\2020\gmail_app\gmail_app_old\gmail_app_old\database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B1D3A26-DED6-4449-A8C6-02530A560858}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AFF1E591-2F57-4D25-971E-CCBAD885B801}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="group_a" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>FIRSTFROMNAME</t>
   </si>
@@ -43,25 +43,19 @@
     <t>PROXY_PASS</t>
   </si>
   <si>
-    <t xml:space="preserve">Adriana </t>
-  </si>
-  <si>
-    <t>Argentina</t>
-  </si>
-  <si>
-    <t>argentinaadriano08@gmail.com</t>
-  </si>
-  <si>
-    <t>dxftsjyntgpahura</t>
-  </si>
-  <si>
-    <t>81.28.96.144:4046</t>
-  </si>
-  <si>
-    <t>hZD3HF2EecZnGtWp</t>
-  </si>
-  <si>
-    <t>YXTAK2bpP9NGzRBS</t>
+    <t>catoirebuster348995@gmail.com</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lozh sfht fvyv uzje </t>
+  </si>
+  <si>
+    <t>185.125.171.131:4022</t>
+  </si>
+  <si>
+    <t>5Gre3gC3S1si</t>
+  </si>
+  <si>
+    <t>Vf0GMX6qc8e6</t>
   </si>
 </sst>
 </file>
@@ -895,19 +889,19 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="3" max="3" width="24" customWidth="1"/>
-    <col min="4" max="4" width="25.6640625" customWidth="1"/>
-    <col min="5" max="5" width="23.88671875" customWidth="1"/>
-    <col min="6" max="6" width="19.33203125" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" customWidth="1"/>
+    <col min="4" max="4" width="25.7109375" customWidth="1"/>
+    <col min="5" max="5" width="23.85546875" customWidth="1"/>
+    <col min="6" max="6" width="19.28515625" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -930,34 +924,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="F2" t="s">
         <v>10</v>
       </c>
-      <c r="E2" t="s">
+      <c r="G2" t="s">
         <v>11</v>
-      </c>
-      <c r="F2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G2" t="s">
-        <v>13</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="C2" r:id="rId1" xr:uid="{CBA38B4A-71B6-4C91-B9D3-1E2AB1824182}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId2"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>